<commit_message>
hpa 0.2.1 adding bundle
</commit_message>
<xml_diff>
--- a/StructureDefinition-Condition-HPA.xlsx
+++ b/StructureDefinition-Condition-HPA.xlsx
@@ -27,13 +27,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://etatunghpa.com/StructureDefinition/Condition-HPA</t>
+    <t>https://twhpa.tsti.com/StructureDefinition/Condition-HPA</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -1028,7 +1028,7 @@
     <t>需要參照系統中的一個特定代碼</t>
   </si>
   <si>
-    <t>https://etatunghpa.com/ValueSet/snomed-medical-history-code</t>
+    <t>https://twhpa.tsti.com/ValueSet/snomed-medical-history-code</t>
   </si>
   <si>
     <t>Coding.code</t>
@@ -1144,7 +1144,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://etatunghpa.com/StructureDefinition/Patient-HPA)
+    <t xml:space="preserve">Reference(https://twhpa.tsti.com/StructureDefinition/Patient-HPA)
 </t>
   </si>
   <si>
@@ -1172,7 +1172,7 @@
     <t>Condition.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://etatunghpa.com/StructureDefinition/Encounter-HPA)
+    <t xml:space="preserve">Reference(https://twhpa.tsti.com/StructureDefinition/Encounter-HPA)
 </t>
   </si>
   <si>
@@ -1291,7 +1291,7 @@
     <t>Condition.asserter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://etatunghpa.com/StructureDefinition/Practitioner-HPA)
+    <t xml:space="preserve">Reference(https://twhpa.tsti.com/StructureDefinition/Practitioner-HPA)
 </t>
   </si>
   <si>

</xml_diff>